<commit_message>
complete teacher bulk upload
</commit_message>
<xml_diff>
--- a/resources/bulk_upload_error/teacher_bulk_upload_error_details_for_excel_file.xlsx
+++ b/resources/bulk_upload_error/teacher_bulk_upload_error_details_for_excel_file.xlsx
@@ -77,25 +77,25 @@
     <t>cardid</t>
   </si>
   <si>
-    <t>Ayan</t>
-  </si>
-  <si>
-    <t>kaur</t>
-  </si>
-  <si>
-    <t>auan.kaur@test.com</t>
-  </si>
-  <si>
-    <t>10.10.1977</t>
-  </si>
-  <si>
-    <t>10.10.2016</t>
+    <t>merio</t>
+  </si>
+  <si>
+    <t>aloni</t>
+  </si>
+  <si>
+    <t>merio@test.com</t>
+  </si>
+  <si>
+    <t>10.10.1988</t>
+  </si>
+  <si>
+    <t>10.10.2015</t>
   </si>
   <si>
     <t>Teacher</t>
   </si>
   <si>
-    <t>mcom</t>
+    <t>c com</t>
   </si>
   <si>
     <t>commerce</t>
@@ -104,19 +104,19 @@
     <t>male</t>
   </si>
   <si>
-    <t>A+</t>
-  </si>
-  <si>
-    <t>kudi</t>
+    <t>B+</t>
+  </si>
+  <si>
+    <t>nehru park</t>
   </si>
   <si>
     <t>india</t>
   </si>
   <si>
-    <t>rajsthan</t>
-  </si>
-  <si>
-    <t>jodhpur</t>
+    <t>rajasthan</t>
+  </si>
+  <si>
+    <t>pali</t>
   </si>
 </sst>
 </file>
@@ -533,7 +533,7 @@
         <v>21</v>
       </c>
       <c r="C2">
-        <v>252415242</v>
+        <v>8245615232</v>
       </c>
       <c r="D2" t="s">
         <v>22</v>
@@ -554,7 +554,7 @@
         <v>27</v>
       </c>
       <c r="J2">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="K2" t="s">
         <v>28</v>
@@ -575,13 +575,13 @@
         <v>33</v>
       </c>
       <c r="Q2">
-        <v>342001</v>
+        <v>352001</v>
       </c>
       <c r="R2">
-        <v>45142526</v>
+        <v>5245252</v>
       </c>
       <c r="S2">
-        <v>415245</v>
+        <v>415245263</v>
       </c>
     </row>
   </sheetData>

</xml_diff>